<commit_message>
Changes to be committed: 	modified:   delegaciones.xlsx 	modified:   generador.py
</commit_message>
<xml_diff>
--- a/delegaciones.xlsx
+++ b/delegaciones.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C47866-4188-491B-AA21-B5B4EF4C5910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="4440" yWindow="2400" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>NOMBRE DELEGACION</t>
   </si>
@@ -36,25 +37,22 @@
     <t>PARTIDO</t>
   </si>
   <si>
-    <t>LANUS - SECCION SEGUNDA</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>99909</t>
-  </si>
-  <si>
-    <t>LANUS OESTE</t>
-  </si>
-  <si>
-    <t>LANUS</t>
+    <t>MARCELINO UGARTE</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>9 DE JULIO</t>
+  </si>
+  <si>
+    <t>99906</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,30 +125,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -433,11 +425,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,58 +464,58 @@
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>9</v>
+      <c r="E2" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -544,7 +536,7 @@
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
+      <c r="B12" s="6"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
@@ -553,39 +545,39 @@
       <c r="E13" s="4"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
+      <c r="B17" s="6"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="D22" s="8"/>
+      <c r="B22" s="6"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="8"/>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="8"/>
+      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="8"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="8"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
+      <c r="B27" s="6"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
+      <c r="B32" s="6"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="A37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="A38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>